<commit_message>
added labels and stuff
</commit_message>
<xml_diff>
--- a/trials.xlsx
+++ b/trials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenders/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenders/Desktop/NN/ML_rain_prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF5903B-09D6-AD40-B08C-A65B0EC515A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CB1FF1-A7E0-EE42-9D31-D30F17F542EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="22860" windowHeight="17220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="22860" windowHeight="17220" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="no_pca" sheetId="5" r:id="rId1"/>
@@ -19,6 +19,12 @@
     <sheet name="3_comps" sheetId="2" r:id="rId4"/>
     <sheet name="2_comps" sheetId="1" r:id="rId5"/>
     <sheet name="1_comp" sheetId="6" r:id="rId6"/>
+    <sheet name="oct_4_comps" sheetId="8" r:id="rId7"/>
+    <sheet name="nov_4_comps" sheetId="9" r:id="rId8"/>
+    <sheet name="dec_4_comps" sheetId="10" r:id="rId9"/>
+    <sheet name="jan_4_comps" sheetId="12" r:id="rId10"/>
+    <sheet name="feb_4_comps" sheetId="13" r:id="rId11"/>
+    <sheet name="mar_4_comps" sheetId="15" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="16">
   <si>
     <t>Cluster 1</t>
   </si>
@@ -1204,6 +1210,762 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E247480-D0A3-B74F-8A70-E10DF8B3253A}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.38480000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:J8" si="0">AVERAGE(C2:C6)</f>
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33880000000000005</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30779999999999996</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49239999999999995</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.35420000000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(B8:J8)</f>
+        <v>0.33357777777777775</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{998F9E2A-E00D-154C-AA5A-2BCAB32169E5}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="J2" s="2">
+        <v>7.6899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.27717999999999998</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:J8" si="0">AVERAGE(C2:C6)</f>
+        <v>0.20020000000000002</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38480000000000003</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30800000000000005</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20017999999999997</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21560000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.49220000000000008</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23098000000000002</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(B8:J8)</f>
+        <v>0.28223777777777781</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E94E97-A98C-C54E-BF99-85C863DAAEDA}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:J8" si="0">AVERAGE(C2:C6)</f>
+        <v>0.20020000000000002</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26178000000000001</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52300000000000002</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23098000000000002</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.35419999999999996</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41580000000000006</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(B8:J8)</f>
+        <v>0.3505955555555556</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K8"/>
@@ -1460,7 +2222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1712,7 +2474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:J6"/>
     </sheetView>
   </sheetViews>
@@ -1965,7 +2727,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2462,4 +3224,760 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289B8328-D154-A647-A3FC-A411729B804F}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.61538461538461497</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.76923076923076905</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.69230769230769196</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.44615384615384562</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:J8" si="0">AVERAGE(C2:C6)</f>
+        <v>0.2923076923076916</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5384615384615381</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.44615384615384562</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56923076923076876</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55384615384615343</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.46153846153846095</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.36923076923076853</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.55384615384615343</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(B8:J8)</f>
+        <v>0.47008547008546953</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2220773A-7014-9345-ADF2-B6146FF34418}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7.6899999999999996E-2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.154</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.23100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.26180000000000003</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:J8" si="0">AVERAGE(C2:C6)</f>
+        <v>0.33879999999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.308</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20020000000000002</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29258000000000001</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33879999999999999</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41539999999999999</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2772</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(B8:J8)</f>
+        <v>0.2959755555555556</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49AA037-E8DA-7C4B-8F17-F3D6767A7B73}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7.69230769230769E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.46153846153846101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="E6" s="1">
+        <v>7.69230769230769E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.15384615384615299</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.38461538461538403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1">
+        <f>AVERAGE(B2:B6)</f>
+        <v>0.43076923076923024</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:J8" si="0">AVERAGE(C2:C6)</f>
+        <v>0.32307692307692237</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.27692307692307622</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29230769230769182</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4153846153846148</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.30769230769230699</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.21538461538461456</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29230769230769182</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="K8" s="1">
+        <f>AVERAGE(B8:J8)</f>
+        <v>0.32649572649572589</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>